<commit_message>
MOS-21370 Updated the Registration Processor Validations
Updated the Validations
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_RegistrationProcessor_ListOfValidations_03Mar'19.xlsx
+++ b/docs/requirements/MOSIP_RegistrationProcessor_ListOfValidations_03Mar'19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Registration Processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC12CFF-720C-4180-9FCC-B1A4811BFBB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3341325F-DFAB-41CF-8F47-62FF27F77E61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{4DB839CF-1097-42B0-B997-B047BD24E725}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="All Validations" sheetId="1" r:id="rId1"/>
     <sheet name="Note" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Validations'!$A$2:$H$2</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="72">
   <si>
     <t>Stage Name</t>
   </si>
@@ -42,9 +45,6 @@
     <t>Configurable</t>
   </si>
   <si>
-    <t>Failure Outcome</t>
-  </si>
-  <si>
     <t>Packet Receiver Stage</t>
   </si>
   <si>
@@ -102,24 +102,6 @@
     <t>OSI Validator Stage</t>
   </si>
   <si>
-    <t>Valdiate Center wrt. Packet Creation Date for Active Center</t>
-  </si>
-  <si>
-    <t>Validate Machine wrt. Packet Creation Date for Active Machines</t>
-  </si>
-  <si>
-    <t>Validate Officer wrt. Packet Creation Date for Active/Blacklisted Officer</t>
-  </si>
-  <si>
-    <t>Validate Supervisor wrt. Packet Creation Date for Active/Blacklisted Supervisor</t>
-  </si>
-  <si>
-    <t>Validate Officer-Center-Machine Mapping wrt. Packet Creation Date</t>
-  </si>
-  <si>
-    <t>Validate Supervisor-Center-Machine Mapping wrt. Packet Creation Date</t>
-  </si>
-  <si>
     <t>Reject the Packet, Notify Resident</t>
   </si>
   <si>
@@ -135,15 +117,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t xml:space="preserve">Validate if Packet was Created on a Holiday wrt. Packet Creation Date </t>
-  </si>
-  <si>
-    <t>Validate Registered Devices wrt. Packet Creation Date</t>
-  </si>
-  <si>
-    <t>Validate Registered Devices-Center Mapping wrt. Packet Creation Date</t>
-  </si>
-  <si>
     <t>Validate if Atleast One Officer/Supervisor is Present in Packet</t>
   </si>
   <si>
@@ -220,6 +193,63 @@
   </si>
   <si>
     <t>Registration Processor</t>
+  </si>
+  <si>
+    <t>Validate Officer Not Found</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>Validate Machine Not Found</t>
+  </si>
+  <si>
+    <t>Validate if Center Not Found</t>
+  </si>
+  <si>
+    <t>Validate Supervisor Not Found</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Current Failure Outcome</t>
+  </si>
+  <si>
+    <t>Valdiate if Center was Active during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Machine was Active during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Officer was Active/Not Blacklisted during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Supervisor was Active/Not Blacklisted during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Officer-Center-Machine Mapping is Present during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Supervisor-Center-Machine Mapping is Present during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate if Packet was Created on a Holiday during Packet Creation DateTime </t>
+  </si>
+  <si>
+    <t>Validate Registered Devices during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Validate Registered Devices-Center Mapping during Packet Creation DateTime</t>
+  </si>
+  <si>
+    <t>Future Outcomes</t>
+  </si>
+  <si>
+    <t>Re-Send</t>
   </si>
 </sst>
 </file>
@@ -738,7 +768,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -757,6 +787,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1113,13 +1146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB5DF25-5B43-4965-AE6B-860EF1FD71B1}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1128,15 +1161,16 @@
     <col min="2" max="2" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.08984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="86.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.36328125" style="1"/>
+    <col min="5" max="5" width="13.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="86.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.36328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1144,13 +1178,14 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -1158,835 +1193,1073 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <f>$A$3</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <f t="shared" ref="B4:B9" si="0">$A$3</f>
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <f>$A$10</f>
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <f>$A$10</f>
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="G12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <f>$A$17</f>
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B18" s="2">
+        <f>$A$17</f>
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B19" s="2">
+        <f>$A$19</f>
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f>$A$19</f>
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <f>$A$22</f>
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" ref="B23:B25" si="1">$A$22</f>
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <f>$A$22</f>
+        <v>20</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <f>$A$27</f>
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <f>$A$27</f>
+        <v>25</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1">
-        <f>$A$20</f>
-        <v>18</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <f t="shared" ref="B21:B24" si="1">$A$20</f>
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="H29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1">
-        <f>$A$26</f>
-        <v>24</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1">
-        <f>$A$26</f>
-        <v>24</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <f>$A$30</f>
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+      <c r="B31" s="2">
+        <f>$A$30</f>
+        <v>28</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
-        <f t="shared" ref="B31:B33" si="2">$A$30</f>
+      <c r="E32" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="H32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
+      <c r="B33" s="2"/>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
-        <f t="shared" si="2"/>
+      <c r="E33" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
+      <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <f>$A$34</f>
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" ref="B35:B37" si="2">$A$34</f>
+        <v>32</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2">
+        <f>$A$38</f>
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2">
+        <f>$A$38</f>
+        <v>36</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2">
+        <f>$A$40</f>
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2">
+        <f>$A$40</f>
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="E42" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1">
-        <f>$A$34</f>
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1">
-        <f>$A$36</f>
-        <v>34</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1">
-        <f>$A$36</f>
-        <v>34</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>35</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A2:H2" xr:uid="{265B7848-CA32-4A8D-B5BB-2DB4160A8F58}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>